<commit_message>
More updates to Bestiary view
+ Added Subterranean Orientation K/S, which had somehow gotten missed before(!)
+ Added ability to vary STEEP via randomization where K/S areas are present and ranges are given
+ Added Outstanding K/S section to Bestiary view
+ Added repeating sections for multiple movement types
* Various cosmetic changes to Bestiary view
+Finished all remaining heka automatic computations
</commit_message>
<xml_diff>
--- a/DangerousJourneys-Mythus/accessories/roll20_import_generator2.xlsx
+++ b/DangerousJourneys-Mythus/accessories/roll20_import_generator2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\apbrezen\Documents\GitHub\DangerousJourneys-Mythus\accessories\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFC11E74-4E13-49A7-81CE-090FAF6442BC}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59F3F9E9-8E08-48FA-9F6B-FE77B93BE4B2}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="45" windowWidth="29040" windowHeight="16440" activeTab="5" xr2:uid="{9DECB17E-D9C9-49D2-8AD7-DCA09A433D93}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1527" uniqueCount="754">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1528" uniqueCount="754">
   <si>
     <t>Weapon Name</t>
   </si>
@@ -4026,10 +4026,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F535ADF2-5DDB-4A56-A3F4-DC4F3A8635C8}">
-  <dimension ref="A1:V589"/>
+  <dimension ref="A1:V590"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="A56" sqref="A56"/>
+    <sheetView topLeftCell="A551" workbookViewId="0">
+      <selection activeCell="A584" sqref="A584"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9873,7 +9873,7 @@
       <c r="B394" s="8"/>
       <c r="I394" s="8"/>
       <c r="U394" t="str">
-        <f t="shared" ref="U394:U457" si="11">IF(C394=1,CONCATENATE(A394,"_kstoggle^1|",A394,"_steep^",D394,"|"),"")</f>
+        <f t="shared" ref="U394:U458" si="11">IF(C394=1,CONCATENATE(A394,"_kstoggle^1|",A394,"_steep^",D394,"|"),"")</f>
         <v/>
       </c>
       <c r="V394" t="str">
@@ -9930,7 +9930,7 @@
         <v/>
       </c>
       <c r="V397" t="str">
-        <f t="shared" ref="V397:V460" si="12">IF(G397=1,CONCATENATE(F397,"_has^1",IF(H397=1,CONCATENATE("|",F397,"_spec^1"),),IF(I397=1,CONCATENATE("|",F397,"_proof^1"),)),"")</f>
+        <f t="shared" ref="V397:V461" si="12">IF(G397=1,CONCATENATE(F397,"_has^1",IF(H397=1,CONCATENATE("|",F397,"_spec^1"),),IF(I397=1,CONCATENATE("|",F397,"_proof^1"),)),"")</f>
         <v/>
       </c>
     </row>
@@ -10680,7 +10680,7 @@
     </row>
     <row r="443" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A443" s="8" t="s">
-        <v>333</v>
+        <v>753</v>
       </c>
       <c r="B443" s="8"/>
       <c r="I443" s="8"/>
@@ -10695,7 +10695,7 @@
     </row>
     <row r="444" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A444" s="8" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B444" s="8"/>
       <c r="I444" s="8"/>
@@ -10710,7 +10710,7 @@
     </row>
     <row r="445" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A445" s="8" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B445" s="8"/>
       <c r="I445" s="8"/>
@@ -10725,7 +10725,7 @@
     </row>
     <row r="446" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A446" s="8" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B446" s="8"/>
       <c r="I446" s="8"/>
@@ -10740,7 +10740,7 @@
     </row>
     <row r="447" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A447" s="8" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B447" s="8"/>
       <c r="I447" s="8"/>
@@ -10755,19 +10755,13 @@
     </row>
     <row r="448" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A448" s="8" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B448" s="8"/>
-      <c r="C448">
-        <v>1</v>
-      </c>
-      <c r="D448">
-        <v>57</v>
-      </c>
       <c r="I448" s="8"/>
       <c r="U448" t="str">
         <f t="shared" si="11"/>
-        <v>weaponsspecialskill_kstoggle^1|weaponsspecialskill_steep^57|</v>
+        <v/>
       </c>
       <c r="V448" t="str">
         <f t="shared" si="12"/>
@@ -10775,26 +10769,24 @@
       </c>
     </row>
     <row r="449" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A449" s="8"/>
-      <c r="B449" t="s">
-        <v>687</v>
-      </c>
-      <c r="E449" t="s">
-        <v>723</v>
-      </c>
-      <c r="F449" s="8" t="s">
-        <v>596</v>
-      </c>
-      <c r="G449">
+      <c r="A449" s="8" t="s">
+        <v>338</v>
+      </c>
+      <c r="B449" s="8"/>
+      <c r="C449">
         <v>1</v>
       </c>
+      <c r="D449">
+        <v>57</v>
+      </c>
+      <c r="I449" s="8"/>
       <c r="U449" t="str">
         <f t="shared" si="11"/>
-        <v/>
+        <v>weaponsspecialskill_kstoggle^1|weaponsspecialskill_steep^57|</v>
       </c>
       <c r="V449" t="str">
         <f t="shared" si="12"/>
-        <v>florentine_has^1</v>
+        <v/>
       </c>
     </row>
     <row r="450" spans="1:22" x14ac:dyDescent="0.25">
@@ -10803,10 +10795,10 @@
         <v>687</v>
       </c>
       <c r="E450" t="s">
-        <v>724</v>
-      </c>
-      <c r="F450" t="s">
-        <v>597</v>
+        <v>723</v>
+      </c>
+      <c r="F450" s="8" t="s">
+        <v>596</v>
       </c>
       <c r="G450">
         <v>1</v>
@@ -10817,7 +10809,7 @@
       </c>
       <c r="V450" t="str">
         <f t="shared" si="12"/>
-        <v>fastdraw_has^1</v>
+        <v>florentine_has^1</v>
       </c>
     </row>
     <row r="451" spans="1:22" x14ac:dyDescent="0.25">
@@ -10826,10 +10818,10 @@
         <v>687</v>
       </c>
       <c r="E451" t="s">
-        <v>21</v>
+        <v>724</v>
       </c>
       <c r="F451" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="G451">
         <v>1</v>
@@ -10840,7 +10832,7 @@
       </c>
       <c r="V451" t="str">
         <f t="shared" si="12"/>
-        <v>specifictarget_has^1</v>
+        <v>fastdraw_has^1</v>
       </c>
     </row>
     <row r="452" spans="1:22" x14ac:dyDescent="0.25">
@@ -10849,10 +10841,10 @@
         <v>687</v>
       </c>
       <c r="E452" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="F452" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="G452">
         <v>1</v>
@@ -10863,27 +10855,35 @@
       </c>
       <c r="V452" t="str">
         <f t="shared" si="12"/>
-        <v>blindfighting_has^1</v>
+        <v>specifictarget_has^1</v>
       </c>
     </row>
     <row r="453" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A453" s="8" t="s">
-        <v>127</v>
-      </c>
-      <c r="B453" s="8"/>
-      <c r="I453" s="8"/>
+      <c r="A453" s="8"/>
+      <c r="B453" t="s">
+        <v>687</v>
+      </c>
+      <c r="E453" t="s">
+        <v>29</v>
+      </c>
+      <c r="F453" t="s">
+        <v>599</v>
+      </c>
+      <c r="G453">
+        <v>1</v>
+      </c>
       <c r="U453" t="str">
         <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="V453" t="str">
         <f t="shared" si="12"/>
-        <v/>
+        <v>blindfighting_has^1</v>
       </c>
     </row>
     <row r="454" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A454" s="8" t="s">
-        <v>339</v>
+        <v>127</v>
       </c>
       <c r="B454" s="8"/>
       <c r="I454" s="8"/>
@@ -10897,11 +10897,10 @@
       </c>
     </row>
     <row r="455" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A455" s="8"/>
+      <c r="A455" s="8" t="s">
+        <v>339</v>
+      </c>
       <c r="B455" s="8"/>
-      <c r="F455" s="8" t="s">
-        <v>600</v>
-      </c>
       <c r="I455" s="8"/>
       <c r="U455" t="str">
         <f t="shared" si="11"/>
@@ -10915,8 +10914,8 @@
     <row r="456" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A456" s="8"/>
       <c r="B456" s="8"/>
-      <c r="F456" t="s">
-        <v>601</v>
+      <c r="F456" s="8" t="s">
+        <v>600</v>
       </c>
       <c r="I456" s="8"/>
       <c r="U456" t="str">
@@ -10932,7 +10931,7 @@
       <c r="A457" s="8"/>
       <c r="B457" s="8"/>
       <c r="F457" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="I457" s="8"/>
       <c r="U457" t="str">
@@ -10948,11 +10947,11 @@
       <c r="A458" s="8"/>
       <c r="B458" s="8"/>
       <c r="F458" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="I458" s="8"/>
       <c r="U458" t="str">
-        <f t="shared" ref="U458:U521" si="13">IF(C458=1,CONCATENATE(A458,"_kstoggle^1|",A458,"_steep^",D458,"|"),"")</f>
+        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="V458" t="str">
@@ -10964,11 +10963,11 @@
       <c r="A459" s="8"/>
       <c r="B459" s="8"/>
       <c r="F459" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="I459" s="8"/>
       <c r="U459" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" ref="U459:U522" si="13">IF(C459=1,CONCATENATE(A459,"_kstoggle^1|",A459,"_steep^",D459,"|"),"")</f>
         <v/>
       </c>
       <c r="V459" t="str">
@@ -10980,7 +10979,7 @@
       <c r="A460" s="8"/>
       <c r="B460" s="8"/>
       <c r="F460" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="I460" s="8"/>
       <c r="U460" t="str">
@@ -10996,7 +10995,7 @@
       <c r="A461" s="8"/>
       <c r="B461" s="8"/>
       <c r="F461" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="I461" s="8"/>
       <c r="U461" t="str">
@@ -11004,7 +11003,7 @@
         <v/>
       </c>
       <c r="V461" t="str">
-        <f t="shared" ref="V461:V524" si="14">IF(G461=1,CONCATENATE(F461,"_has^1",IF(H461=1,CONCATENATE("|",F461,"_spec^1"),),IF(I461=1,CONCATENATE("|",F461,"_proof^1"),)),"")</f>
+        <f t="shared" si="12"/>
         <v/>
       </c>
     </row>
@@ -11012,7 +11011,7 @@
       <c r="A462" s="8"/>
       <c r="B462" s="8"/>
       <c r="F462" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="I462" s="8"/>
       <c r="U462" t="str">
@@ -11020,7 +11019,7 @@
         <v/>
       </c>
       <c r="V462" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" ref="V462:V525" si="14">IF(G462=1,CONCATENATE(F462,"_has^1",IF(H462=1,CONCATENATE("|",F462,"_spec^1"),),IF(I462=1,CONCATENATE("|",F462,"_proof^1"),)),"")</f>
         <v/>
       </c>
     </row>
@@ -11028,7 +11027,7 @@
       <c r="A463" s="8"/>
       <c r="B463" s="8"/>
       <c r="F463" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="I463" s="8"/>
       <c r="U463" t="str">
@@ -11044,7 +11043,7 @@
       <c r="A464" s="8"/>
       <c r="B464" s="8"/>
       <c r="F464" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="I464" s="8"/>
       <c r="U464" t="str">
@@ -11060,7 +11059,7 @@
       <c r="A465" s="8"/>
       <c r="B465" s="8"/>
       <c r="F465" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="I465" s="8"/>
       <c r="U465" t="str">
@@ -11076,7 +11075,7 @@
       <c r="A466" s="8"/>
       <c r="B466" s="8"/>
       <c r="F466" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="I466" s="8"/>
       <c r="U466" t="str">
@@ -11092,7 +11091,7 @@
       <c r="A467" s="8"/>
       <c r="B467" s="8"/>
       <c r="F467" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="I467" s="8"/>
       <c r="U467" t="str">
@@ -11108,7 +11107,7 @@
       <c r="A468" s="8"/>
       <c r="B468" s="8"/>
       <c r="F468" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="I468" s="8"/>
       <c r="U468" t="str">
@@ -11121,10 +11120,11 @@
       </c>
     </row>
     <row r="469" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A469" s="8" t="s">
-        <v>129</v>
-      </c>
+      <c r="A469" s="8"/>
       <c r="B469" s="8"/>
+      <c r="F469" t="s">
+        <v>613</v>
+      </c>
       <c r="I469" s="8"/>
       <c r="U469" t="str">
         <f t="shared" si="13"/>
@@ -11137,7 +11137,7 @@
     </row>
     <row r="470" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A470" s="8" t="s">
-        <v>340</v>
+        <v>129</v>
       </c>
       <c r="B470" s="8"/>
       <c r="I470" s="8"/>
@@ -11151,11 +11151,10 @@
       </c>
     </row>
     <row r="471" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A471" s="8"/>
+      <c r="A471" s="8" t="s">
+        <v>340</v>
+      </c>
       <c r="B471" s="8"/>
-      <c r="F471" s="8" t="s">
-        <v>614</v>
-      </c>
       <c r="I471" s="8"/>
       <c r="U471" t="str">
         <f t="shared" si="13"/>
@@ -11169,8 +11168,8 @@
     <row r="472" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A472" s="8"/>
       <c r="B472" s="8"/>
-      <c r="F472" t="s">
-        <v>615</v>
+      <c r="F472" s="8" t="s">
+        <v>614</v>
       </c>
       <c r="I472" s="8"/>
       <c r="U472" t="str">
@@ -11186,7 +11185,7 @@
       <c r="A473" s="8"/>
       <c r="B473" s="8"/>
       <c r="F473" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="I473" s="8"/>
       <c r="U473" t="str">
@@ -11202,7 +11201,7 @@
       <c r="A474" s="8"/>
       <c r="B474" s="8"/>
       <c r="F474" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="I474" s="8"/>
       <c r="U474" t="str">
@@ -11218,7 +11217,7 @@
       <c r="A475" s="8"/>
       <c r="B475" s="8"/>
       <c r="F475" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="I475" s="8"/>
       <c r="U475" t="str">
@@ -11234,7 +11233,7 @@
       <c r="A476" s="8"/>
       <c r="B476" s="8"/>
       <c r="F476" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="I476" s="8"/>
       <c r="U476" t="str">
@@ -11250,7 +11249,7 @@
       <c r="A477" s="8"/>
       <c r="B477" s="8"/>
       <c r="F477" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="I477" s="8"/>
       <c r="U477" t="str">
@@ -11266,7 +11265,7 @@
       <c r="A478" s="8"/>
       <c r="B478" s="8"/>
       <c r="F478" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="I478" s="8"/>
       <c r="U478" t="str">
@@ -11282,7 +11281,7 @@
       <c r="A479" s="8"/>
       <c r="B479" s="8"/>
       <c r="F479" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="I479" s="8"/>
       <c r="U479" t="str">
@@ -11298,7 +11297,7 @@
       <c r="A480" s="8"/>
       <c r="B480" s="8"/>
       <c r="F480" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="I480" s="8"/>
       <c r="U480" t="str">
@@ -11314,7 +11313,7 @@
       <c r="A481" s="8"/>
       <c r="B481" s="8"/>
       <c r="F481" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="I481" s="8"/>
       <c r="U481" t="str">
@@ -11330,7 +11329,7 @@
       <c r="A482" s="8"/>
       <c r="B482" s="8"/>
       <c r="F482" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="I482" s="8"/>
       <c r="U482" t="str">
@@ -11343,10 +11342,11 @@
       </c>
     </row>
     <row r="483" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A483" s="8" t="s">
-        <v>341</v>
-      </c>
+      <c r="A483" s="8"/>
       <c r="B483" s="8"/>
+      <c r="F483" t="s">
+        <v>625</v>
+      </c>
       <c r="I483" s="8"/>
       <c r="U483" t="str">
         <f t="shared" si="13"/>
@@ -11359,7 +11359,7 @@
     </row>
     <row r="484" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A484" s="8" t="s">
-        <v>130</v>
+        <v>341</v>
       </c>
       <c r="B484" s="8"/>
       <c r="I484" s="8"/>
@@ -11374,7 +11374,7 @@
     </row>
     <row r="485" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A485" s="8" t="s">
-        <v>342</v>
+        <v>130</v>
       </c>
       <c r="B485" s="8"/>
       <c r="I485" s="8"/>
@@ -11389,7 +11389,7 @@
     </row>
     <row r="486" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A486" s="8" t="s">
-        <v>131</v>
+        <v>342</v>
       </c>
       <c r="B486" s="8"/>
       <c r="I486" s="8"/>
@@ -11403,11 +11403,10 @@
       </c>
     </row>
     <row r="487" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A487" s="8"/>
+      <c r="A487" s="8" t="s">
+        <v>131</v>
+      </c>
       <c r="B487" s="8"/>
-      <c r="F487" s="8" t="s">
-        <v>626</v>
-      </c>
       <c r="I487" s="8"/>
       <c r="U487" t="str">
         <f t="shared" si="13"/>
@@ -11421,8 +11420,8 @@
     <row r="488" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A488" s="8"/>
       <c r="B488" s="8"/>
-      <c r="F488" t="s">
-        <v>627</v>
+      <c r="F488" s="8" t="s">
+        <v>626</v>
       </c>
       <c r="I488" s="8"/>
       <c r="U488" t="str">
@@ -11438,7 +11437,7 @@
       <c r="A489" s="8"/>
       <c r="B489" s="8"/>
       <c r="F489" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="I489" s="8"/>
       <c r="U489" t="str">
@@ -11454,7 +11453,7 @@
       <c r="A490" s="8"/>
       <c r="B490" s="8"/>
       <c r="F490" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="I490" s="8"/>
       <c r="U490" t="str">
@@ -11470,7 +11469,7 @@
       <c r="A491" s="8"/>
       <c r="B491" s="8"/>
       <c r="F491" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="I491" s="8"/>
       <c r="U491" t="str">
@@ -11483,10 +11482,11 @@
       </c>
     </row>
     <row r="492" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A492" s="8" t="s">
-        <v>138</v>
-      </c>
+      <c r="A492" s="8"/>
       <c r="B492" s="8"/>
+      <c r="F492" t="s">
+        <v>630</v>
+      </c>
       <c r="I492" s="8"/>
       <c r="U492" t="str">
         <f t="shared" si="13"/>
@@ -11499,7 +11499,7 @@
     </row>
     <row r="493" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A493" s="8" t="s">
-        <v>104</v>
+        <v>138</v>
       </c>
       <c r="B493" s="8"/>
       <c r="I493" s="8"/>
@@ -11513,11 +11513,10 @@
       </c>
     </row>
     <row r="494" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A494" s="8"/>
+      <c r="A494" s="8" t="s">
+        <v>104</v>
+      </c>
       <c r="B494" s="8"/>
-      <c r="F494" s="8" t="s">
-        <v>631</v>
-      </c>
       <c r="I494" s="8"/>
       <c r="U494" t="str">
         <f t="shared" si="13"/>
@@ -11531,8 +11530,8 @@
     <row r="495" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A495" s="8"/>
       <c r="B495" s="8"/>
-      <c r="F495" t="s">
-        <v>632</v>
+      <c r="F495" s="8" t="s">
+        <v>631</v>
       </c>
       <c r="I495" s="8"/>
       <c r="U495" t="str">
@@ -11548,7 +11547,7 @@
       <c r="A496" s="8"/>
       <c r="B496" s="8"/>
       <c r="F496" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="I496" s="8"/>
       <c r="U496" t="str">
@@ -11564,7 +11563,7 @@
       <c r="A497" s="8"/>
       <c r="B497" s="8"/>
       <c r="F497" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="I497" s="8"/>
       <c r="U497" t="str">
@@ -11580,7 +11579,7 @@
       <c r="A498" s="8"/>
       <c r="B498" s="8"/>
       <c r="F498" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="I498" s="8"/>
       <c r="U498" t="str">
@@ -11596,7 +11595,7 @@
       <c r="A499" s="8"/>
       <c r="B499" s="8"/>
       <c r="F499" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="I499" s="8"/>
       <c r="U499" t="str">
@@ -11609,10 +11608,11 @@
       </c>
     </row>
     <row r="500" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A500" s="8" t="s">
-        <v>140</v>
-      </c>
+      <c r="A500" s="8"/>
       <c r="B500" s="8"/>
+      <c r="F500" t="s">
+        <v>636</v>
+      </c>
       <c r="I500" s="8"/>
       <c r="U500" t="str">
         <f t="shared" si="13"/>
@@ -11625,7 +11625,7 @@
     </row>
     <row r="501" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A501" s="8" t="s">
-        <v>343</v>
+        <v>140</v>
       </c>
       <c r="B501" s="8"/>
       <c r="I501" s="8"/>
@@ -11640,7 +11640,7 @@
     </row>
     <row r="502" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A502" s="8" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="B502" s="8"/>
       <c r="I502" s="8"/>
@@ -11654,11 +11654,10 @@
       </c>
     </row>
     <row r="503" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A503" s="8"/>
+      <c r="A503" s="8" t="s">
+        <v>344</v>
+      </c>
       <c r="B503" s="8"/>
-      <c r="F503" s="8" t="s">
-        <v>637</v>
-      </c>
       <c r="I503" s="8"/>
       <c r="U503" t="str">
         <f t="shared" si="13"/>
@@ -11672,8 +11671,8 @@
     <row r="504" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A504" s="8"/>
       <c r="B504" s="8"/>
-      <c r="F504" t="s">
-        <v>638</v>
+      <c r="F504" s="8" t="s">
+        <v>637</v>
       </c>
       <c r="I504" s="8"/>
       <c r="U504" t="str">
@@ -11689,7 +11688,7 @@
       <c r="A505" s="8"/>
       <c r="B505" s="8"/>
       <c r="F505" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="I505" s="8"/>
       <c r="U505" t="str">
@@ -11705,7 +11704,7 @@
       <c r="A506" s="8"/>
       <c r="B506" s="8"/>
       <c r="F506" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="I506" s="8"/>
       <c r="U506" t="str">
@@ -11721,7 +11720,7 @@
       <c r="A507" s="8"/>
       <c r="B507" s="8"/>
       <c r="F507" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="I507" s="8"/>
       <c r="U507" t="str">
@@ -11734,10 +11733,11 @@
       </c>
     </row>
     <row r="508" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A508" s="8" t="s">
-        <v>345</v>
-      </c>
+      <c r="A508" s="8"/>
       <c r="B508" s="8"/>
+      <c r="F508" t="s">
+        <v>641</v>
+      </c>
       <c r="I508" s="8"/>
       <c r="U508" t="str">
         <f t="shared" si="13"/>
@@ -11750,7 +11750,7 @@
     </row>
     <row r="509" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A509" s="8" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B509" s="8"/>
       <c r="I509" s="8"/>
@@ -11765,7 +11765,7 @@
     </row>
     <row r="510" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A510" s="8" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B510" s="8"/>
       <c r="I510" s="8"/>
@@ -11780,7 +11780,7 @@
     </row>
     <row r="511" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A511" s="8" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B511" s="8"/>
       <c r="I511" s="8"/>
@@ -11795,7 +11795,7 @@
     </row>
     <row r="512" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A512" s="8" t="s">
-        <v>141</v>
+        <v>348</v>
       </c>
       <c r="B512" s="8"/>
       <c r="I512" s="8"/>
@@ -11810,7 +11810,7 @@
     </row>
     <row r="513" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A513" s="8" t="s">
-        <v>349</v>
+        <v>141</v>
       </c>
       <c r="B513" s="8"/>
       <c r="I513" s="8"/>
@@ -11825,7 +11825,7 @@
     </row>
     <row r="514" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A514" s="8" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B514" s="8"/>
       <c r="I514" s="8"/>
@@ -11839,11 +11839,10 @@
       </c>
     </row>
     <row r="515" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A515" s="8"/>
+      <c r="A515" s="8" t="s">
+        <v>350</v>
+      </c>
       <c r="B515" s="8"/>
-      <c r="F515" s="8" t="s">
-        <v>642</v>
-      </c>
       <c r="I515" s="8"/>
       <c r="U515" t="str">
         <f t="shared" si="13"/>
@@ -11857,8 +11856,8 @@
     <row r="516" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A516" s="8"/>
       <c r="B516" s="8"/>
-      <c r="F516" t="s">
-        <v>224</v>
+      <c r="F516" s="8" t="s">
+        <v>642</v>
       </c>
       <c r="I516" s="8"/>
       <c r="U516" t="str">
@@ -11874,7 +11873,7 @@
       <c r="A517" s="8"/>
       <c r="B517" s="8"/>
       <c r="F517" t="s">
-        <v>643</v>
+        <v>224</v>
       </c>
       <c r="I517" s="8"/>
       <c r="U517" t="str">
@@ -11890,7 +11889,7 @@
       <c r="A518" s="8"/>
       <c r="B518" s="8"/>
       <c r="F518" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="I518" s="8"/>
       <c r="U518" t="str">
@@ -11906,7 +11905,7 @@
       <c r="A519" s="8"/>
       <c r="B519" s="8"/>
       <c r="F519" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="I519" s="8"/>
       <c r="U519" t="str">
@@ -11922,7 +11921,7 @@
       <c r="A520" s="8"/>
       <c r="B520" s="8"/>
       <c r="F520" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="I520" s="8"/>
       <c r="U520" t="str">
@@ -11938,7 +11937,7 @@
       <c r="A521" s="8"/>
       <c r="B521" s="8"/>
       <c r="F521" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="I521" s="8"/>
       <c r="U521" t="str">
@@ -11954,11 +11953,11 @@
       <c r="A522" s="8"/>
       <c r="B522" s="8"/>
       <c r="F522" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="I522" s="8"/>
       <c r="U522" t="str">
-        <f t="shared" ref="U522:U579" si="15">IF(C522=1,CONCATENATE(A522,"_kstoggle^1|",A522,"_steep^",D522,"|"),"")</f>
+        <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="V522" t="str">
@@ -11970,11 +11969,11 @@
       <c r="A523" s="8"/>
       <c r="B523" s="8"/>
       <c r="F523" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="I523" s="8"/>
       <c r="U523" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" ref="U523:U580" si="15">IF(C523=1,CONCATENATE(A523,"_kstoggle^1|",A523,"_steep^",D523,"|"),"")</f>
         <v/>
       </c>
       <c r="V523" t="str">
@@ -11986,7 +11985,7 @@
       <c r="A524" s="8"/>
       <c r="B524" s="8"/>
       <c r="F524" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="I524" s="8"/>
       <c r="U524" t="str">
@@ -12002,7 +12001,7 @@
       <c r="A525" s="8"/>
       <c r="B525" s="8"/>
       <c r="F525" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="I525" s="8"/>
       <c r="U525" t="str">
@@ -12010,28 +12009,29 @@
         <v/>
       </c>
       <c r="V525" t="str">
-        <f t="shared" ref="V525:V579" si="16">IF(G525=1,CONCATENATE(F525,"_has^1",IF(H525=1,CONCATENATE("|",F525,"_spec^1"),),IF(I525=1,CONCATENATE("|",F525,"_proof^1"),)),"")</f>
+        <f t="shared" si="14"/>
         <v/>
       </c>
     </row>
     <row r="526" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A526" s="8" t="s">
-        <v>351</v>
-      </c>
+      <c r="A526" s="8"/>
       <c r="B526" s="8"/>
+      <c r="F526" t="s">
+        <v>651</v>
+      </c>
       <c r="I526" s="8"/>
       <c r="U526" t="str">
         <f t="shared" si="15"/>
         <v/>
       </c>
       <c r="V526" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" ref="V526:V580" si="16">IF(G526=1,CONCATENATE(F526,"_has^1",IF(H526=1,CONCATENATE("|",F526,"_spec^1"),),IF(I526=1,CONCATENATE("|",F526,"_proof^1"),)),"")</f>
         <v/>
       </c>
     </row>
     <row r="527" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A527" s="8" t="s">
-        <v>142</v>
+        <v>351</v>
       </c>
       <c r="B527" s="8"/>
       <c r="I527" s="8"/>
@@ -12046,7 +12046,7 @@
     </row>
     <row r="528" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A528" s="8" t="s">
-        <v>352</v>
+        <v>142</v>
       </c>
       <c r="B528" s="8"/>
       <c r="I528" s="8"/>
@@ -12060,11 +12060,10 @@
       </c>
     </row>
     <row r="529" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A529" s="8"/>
+      <c r="A529" s="8" t="s">
+        <v>352</v>
+      </c>
       <c r="B529" s="8"/>
-      <c r="F529" s="8" t="s">
-        <v>652</v>
-      </c>
       <c r="I529" s="8"/>
       <c r="U529" t="str">
         <f t="shared" si="15"/>
@@ -12078,8 +12077,8 @@
     <row r="530" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A530" s="8"/>
       <c r="B530" s="8"/>
-      <c r="F530" t="s">
-        <v>653</v>
+      <c r="F530" s="8" t="s">
+        <v>652</v>
       </c>
       <c r="I530" s="8"/>
       <c r="U530" t="str">
@@ -12095,7 +12094,7 @@
       <c r="A531" s="8"/>
       <c r="B531" s="8"/>
       <c r="F531" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="I531" s="8"/>
       <c r="U531" t="str">
@@ -12111,7 +12110,7 @@
       <c r="A532" s="8"/>
       <c r="B532" s="8"/>
       <c r="F532" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="I532" s="8"/>
       <c r="U532" t="str">
@@ -12127,7 +12126,7 @@
       <c r="A533" s="8"/>
       <c r="B533" s="8"/>
       <c r="F533" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="I533" s="8"/>
       <c r="U533" t="str">
@@ -12140,10 +12139,11 @@
       </c>
     </row>
     <row r="534" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A534" s="8" t="s">
-        <v>143</v>
-      </c>
+      <c r="A534" s="8"/>
       <c r="B534" s="8"/>
+      <c r="F534" t="s">
+        <v>656</v>
+      </c>
       <c r="I534" s="8"/>
       <c r="U534" t="str">
         <f t="shared" si="15"/>
@@ -12156,7 +12156,7 @@
     </row>
     <row r="535" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A535" s="8" t="s">
-        <v>353</v>
+        <v>143</v>
       </c>
       <c r="B535" s="8"/>
       <c r="I535" s="8"/>
@@ -12171,7 +12171,7 @@
     </row>
     <row r="536" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A536" s="8" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B536" s="8"/>
       <c r="I536" s="8"/>
@@ -12186,7 +12186,7 @@
     </row>
     <row r="537" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A537" s="8" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B537" s="8"/>
       <c r="I537" s="8"/>
@@ -12200,11 +12200,10 @@
       </c>
     </row>
     <row r="538" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A538" s="8"/>
+      <c r="A538" s="8" t="s">
+        <v>355</v>
+      </c>
       <c r="B538" s="8"/>
-      <c r="F538" s="8" t="s">
-        <v>657</v>
-      </c>
       <c r="I538" s="8"/>
       <c r="U538" t="str">
         <f t="shared" si="15"/>
@@ -12218,8 +12217,8 @@
     <row r="539" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A539" s="8"/>
       <c r="B539" s="8"/>
-      <c r="F539" t="s">
-        <v>658</v>
+      <c r="F539" s="8" t="s">
+        <v>657</v>
       </c>
       <c r="I539" s="8"/>
       <c r="U539" t="str">
@@ -12235,7 +12234,7 @@
       <c r="A540" s="8"/>
       <c r="B540" s="8"/>
       <c r="F540" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="I540" s="8"/>
       <c r="U540" t="str">
@@ -12251,7 +12250,7 @@
       <c r="A541" s="8"/>
       <c r="B541" s="8"/>
       <c r="F541" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="I541" s="8"/>
       <c r="U541" t="str">
@@ -12267,7 +12266,7 @@
       <c r="A542" s="8"/>
       <c r="B542" s="8"/>
       <c r="F542" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="I542" s="8"/>
       <c r="U542" t="str">
@@ -12283,7 +12282,7 @@
       <c r="A543" s="8"/>
       <c r="B543" s="8"/>
       <c r="F543" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="I543" s="8"/>
       <c r="U543" t="str">
@@ -12299,7 +12298,7 @@
       <c r="A544" s="8"/>
       <c r="B544" s="8"/>
       <c r="F544" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="I544" s="8"/>
       <c r="U544" t="str">
@@ -12315,7 +12314,7 @@
       <c r="A545" s="8"/>
       <c r="B545" s="8"/>
       <c r="F545" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="I545" s="8"/>
       <c r="U545" t="str">
@@ -12331,7 +12330,7 @@
       <c r="A546" s="8"/>
       <c r="B546" s="8"/>
       <c r="F546" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="I546" s="8"/>
       <c r="U546" t="str">
@@ -12347,7 +12346,7 @@
       <c r="A547" s="8"/>
       <c r="B547" s="8"/>
       <c r="F547" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="I547" s="8"/>
       <c r="U547" t="str">
@@ -12363,7 +12362,7 @@
       <c r="A548" s="8"/>
       <c r="B548" s="8"/>
       <c r="F548" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="I548" s="8"/>
       <c r="U548" t="str">
@@ -12379,7 +12378,7 @@
       <c r="A549" s="8"/>
       <c r="B549" s="8"/>
       <c r="F549" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="I549" s="8"/>
       <c r="U549" t="str">
@@ -12395,7 +12394,7 @@
       <c r="A550" s="8"/>
       <c r="B550" s="8"/>
       <c r="F550" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="I550" s="8"/>
       <c r="U550" t="str">
@@ -12411,7 +12410,7 @@
       <c r="A551" s="8"/>
       <c r="B551" s="8"/>
       <c r="F551" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="I551" s="8"/>
       <c r="U551" t="str">
@@ -12427,7 +12426,7 @@
       <c r="A552" s="8"/>
       <c r="B552" s="8"/>
       <c r="F552" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="I552" s="8"/>
       <c r="U552" t="str">
@@ -12443,7 +12442,7 @@
       <c r="A553" s="8"/>
       <c r="B553" s="8"/>
       <c r="F553" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="I553" s="8"/>
       <c r="U553" t="str">
@@ -12459,7 +12458,7 @@
       <c r="A554" s="8"/>
       <c r="B554" s="8"/>
       <c r="F554" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="I554" s="8"/>
       <c r="U554" t="str">
@@ -12475,7 +12474,7 @@
       <c r="A555" s="8"/>
       <c r="B555" s="8"/>
       <c r="F555" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="I555" s="8"/>
       <c r="U555" t="str">
@@ -12491,7 +12490,7 @@
       <c r="A556" s="8"/>
       <c r="B556" s="8"/>
       <c r="F556" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="I556" s="8"/>
       <c r="U556" t="str">
@@ -12504,10 +12503,11 @@
       </c>
     </row>
     <row r="557" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A557" s="8" t="s">
-        <v>356</v>
-      </c>
+      <c r="A557" s="8"/>
       <c r="B557" s="8"/>
+      <c r="F557" t="s">
+        <v>675</v>
+      </c>
       <c r="I557" s="8"/>
       <c r="U557" t="str">
         <f t="shared" si="15"/>
@@ -12519,11 +12519,10 @@
       </c>
     </row>
     <row r="558" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A558" s="8"/>
+      <c r="A558" s="8" t="s">
+        <v>356</v>
+      </c>
       <c r="B558" s="8"/>
-      <c r="F558" s="8" t="s">
-        <v>676</v>
-      </c>
       <c r="I558" s="8"/>
       <c r="U558" t="str">
         <f t="shared" si="15"/>
@@ -12537,8 +12536,8 @@
     <row r="559" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A559" s="8"/>
       <c r="B559" s="8"/>
-      <c r="F559" t="s">
-        <v>677</v>
+      <c r="F559" s="8" t="s">
+        <v>676</v>
       </c>
       <c r="I559" s="8"/>
       <c r="U559" t="str">
@@ -12554,7 +12553,7 @@
       <c r="A560" s="8"/>
       <c r="B560" s="8"/>
       <c r="F560" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="I560" s="8"/>
       <c r="U560" t="str">
@@ -12570,7 +12569,7 @@
       <c r="A561" s="8"/>
       <c r="B561" s="8"/>
       <c r="F561" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="I561" s="8"/>
       <c r="U561" t="str">
@@ -12586,7 +12585,7 @@
       <c r="A562" s="8"/>
       <c r="B562" s="8"/>
       <c r="F562" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="I562" s="8"/>
       <c r="U562" t="str">
@@ -12602,7 +12601,7 @@
       <c r="A563" s="8"/>
       <c r="B563" s="8"/>
       <c r="F563" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="I563" s="8"/>
       <c r="U563" t="str">
@@ -12615,20 +12614,15 @@
       </c>
     </row>
     <row r="564" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A564" s="8" t="s">
-        <v>357</v>
-      </c>
+      <c r="A564" s="8"/>
       <c r="B564" s="8"/>
-      <c r="C564">
-        <v>1</v>
-      </c>
-      <c r="D564">
-        <v>20</v>
+      <c r="F564" t="s">
+        <v>681</v>
       </c>
       <c r="I564" s="8"/>
       <c r="U564" t="str">
         <f t="shared" si="15"/>
-        <v>philosophy_kstoggle^1|philosophy_steep^20|</v>
+        <v/>
       </c>
       <c r="V564" t="str">
         <f t="shared" si="16"/>
@@ -12637,13 +12631,19 @@
     </row>
     <row r="565" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A565" s="8" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="B565" s="8"/>
+      <c r="C565">
+        <v>1</v>
+      </c>
+      <c r="D565">
+        <v>20</v>
+      </c>
       <c r="I565" s="8"/>
       <c r="U565" t="str">
         <f t="shared" si="15"/>
-        <v/>
+        <v>philosophy_kstoggle^1|philosophy_steep^20|</v>
       </c>
       <c r="V565" t="str">
         <f t="shared" si="16"/>
@@ -12652,7 +12652,7 @@
     </row>
     <row r="566" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A566" s="8" t="s">
-        <v>144</v>
+        <v>358</v>
       </c>
       <c r="B566" s="8"/>
       <c r="I566" s="8"/>
@@ -12667,7 +12667,7 @@
     </row>
     <row r="567" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A567" s="8" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B567" s="8"/>
       <c r="I567" s="8"/>
@@ -12682,7 +12682,7 @@
     </row>
     <row r="568" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A568" s="8" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B568" s="8"/>
       <c r="I568" s="8"/>
@@ -12697,7 +12697,7 @@
     </row>
     <row r="569" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A569" s="8" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B569" s="8"/>
       <c r="I569" s="8"/>
@@ -12712,7 +12712,7 @@
     </row>
     <row r="570" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A570" s="8" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B570" s="8"/>
       <c r="I570" s="8"/>
@@ -12727,7 +12727,7 @@
     </row>
     <row r="571" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A571" s="8" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B571" s="8"/>
       <c r="I571" s="8"/>
@@ -12742,7 +12742,7 @@
     </row>
     <row r="572" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A572" s="8" t="s">
-        <v>359</v>
+        <v>149</v>
       </c>
       <c r="B572" s="8"/>
       <c r="I572" s="8"/>
@@ -12757,7 +12757,7 @@
     </row>
     <row r="573" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A573" s="8" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B573" s="8"/>
       <c r="I573" s="8"/>
@@ -12772,7 +12772,7 @@
     </row>
     <row r="574" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A574" s="8" t="s">
-        <v>150</v>
+        <v>360</v>
       </c>
       <c r="B574" s="8"/>
       <c r="I574" s="8"/>
@@ -12787,24 +12787,13 @@
     </row>
     <row r="575" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A575" s="8" t="s">
-        <v>361</v>
-      </c>
-      <c r="B575" t="s">
-        <v>682</v>
-      </c>
-      <c r="C575">
-        <v>1</v>
-      </c>
-      <c r="D575">
-        <v>32</v>
-      </c>
-      <c r="E575" t="s">
-        <v>730</v>
-      </c>
+        <v>150</v>
+      </c>
+      <c r="B575" s="8"/>
       <c r="I575" s="8"/>
       <c r="U575" t="str">
         <f t="shared" si="15"/>
-        <v>streetwise_kstoggle^1|streetwise_steep^32|</v>
+        <v/>
       </c>
       <c r="V575" t="str">
         <f t="shared" si="16"/>
@@ -12813,13 +12802,24 @@
     </row>
     <row r="576" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A576" s="8" t="s">
-        <v>362</v>
-      </c>
-      <c r="B576" s="8"/>
+        <v>361</v>
+      </c>
+      <c r="B576" t="s">
+        <v>682</v>
+      </c>
+      <c r="C576">
+        <v>1</v>
+      </c>
+      <c r="D576">
+        <v>32</v>
+      </c>
+      <c r="E576" t="s">
+        <v>730</v>
+      </c>
       <c r="I576" s="8"/>
       <c r="U576" t="str">
         <f t="shared" si="15"/>
-        <v/>
+        <v>streetwise_kstoggle^1|streetwise_steep^32|</v>
       </c>
       <c r="V576" t="str">
         <f t="shared" si="16"/>
@@ -12828,7 +12828,7 @@
     </row>
     <row r="577" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A577" s="8" t="s">
-        <v>152</v>
+        <v>362</v>
       </c>
       <c r="B577" s="8"/>
       <c r="I577" s="8"/>
@@ -12843,7 +12843,7 @@
     </row>
     <row r="578" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A578" s="8" t="s">
-        <v>363</v>
+        <v>152</v>
       </c>
       <c r="B578" s="8"/>
       <c r="I578" s="8"/>
@@ -12858,7 +12858,7 @@
     </row>
     <row r="579" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A579" s="8" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="B579" s="8"/>
       <c r="I579" s="8"/>
@@ -12871,48 +12871,63 @@
         <v/>
       </c>
     </row>
-    <row r="584" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A584" t="s">
+    <row r="580" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A580" s="8" t="s">
+        <v>364</v>
+      </c>
+      <c r="B580" s="8"/>
+      <c r="I580" s="8"/>
+      <c r="U580" t="str">
+        <f t="shared" si="15"/>
+        <v/>
+      </c>
+      <c r="V580" t="str">
+        <f t="shared" si="16"/>
+        <v/>
+      </c>
+    </row>
+    <row r="585" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A585" t="s">
         <v>692</v>
       </c>
-      <c r="B584" t="str">
+      <c r="B585" t="str">
         <f>CONCATENATE("character_name^",B1,"|","vocation^",B2,"|","vocationtrait^",B3,"|","sec^",B4,"|","attractiveness^",B5,"|","beautyugly^",B6,"|","ap^",B7,"|","joss^",B8,"|","mmcapatt^",B10,"|","mmpowatt^",B11,"|","mmspdatt^",B12,"|","mrcapatt^",B13,"|","mrpowatt^",B14,"|","mrspdatt^",B15,"|","pmcapatt^",B17,"|","pmpowatt^",B18,"|","pmspdatt^",B19,"|","pncapatt^",B20,"|","pnpowatt^",B21,"|","pnspdatt^",B22,"|","smcapatt^",B24,"|","smpowatt^",B25,"|","smspdatt^",B26,"|","spcapatt^",B27,"|","sppowatt^",B28,"|","spspdatt^",B29,"|","traithekamental_toggle^",B31,"|","traithekaphysical_toggle^",B32,"|","traithekaspiritual_toggle^",B33,"|","fpdweomer^",B35,"|","fppriest^",B36,"|","dweomerschool^",B38,"|","priestethos^",B39,"|","vowpact^",B41,"|","vowpact_mult^",B42,"|","age^",B44,"|","sex^",B45,"|","race^",B46,"|","complexion^",B47,"|","handedness^",B48,"|","height^",B49,"|","weight^",B50,"|","build^",B51,"|","eyes^",B52,"|","hair^",B53,"|","physicalother^",B54,"|","personality^",B55,"|","quirks^",B56,"|","quote^",B57,"|","birthdate^",B58,"|","birthplace^",B59,"|","birthrank^",B60,"|","citizenship^",B61,"|","residence^",B62,"|","background^",B63,"|","connections^",B64,"|","networth^",B66,"|","bankaccounts^",B67,"|","cashonhand^",B68,"|","dmi^",B69,"|","possessions1^",B70)</f>
         <v>character_name^Smartypants Hottieface|vocation^Seafarer|vocationtrait^PHYSICAL|sec^5|attractiveness^18|beautyugly^|ap^2|joss^3|mmcapatt^19|mmpowatt^14|mmspdatt^18|mrcapatt^15|mrpowatt^12|mrspdatt^11|pmcapatt^20|pmpowatt^19|pmspdatt^15|pncapatt^19|pnpowatt^18|pnspdatt^17|smcapatt^16|smpowatt^12|smspdatt^11|spcapatt^15|sppowatt^12|spspdatt^13|traithekamental_toggle^0|traithekaphysical_toggle^1|traithekaspiritual_toggle^0|fpdweomer^0|fppriest^0|dweomerschool^|priestethos^|vowpact^|vowpact_mult^1|age^18|sex^Indeed|race^Faerie|complexion^Mocha|handedness^Left|height^5'6"|weight^145 lb.|build^Brickhouse|eyes^Blue|hair^Black|physicalother^Svelte|personality^Savage|quirks^|quote^|birthdate^|birthplace^|birthrank^|citizenship^Detroit|residence^Arizona|background^|connections^|networth^|bankaccounts^|cashonhand^|dmi^|possessions1^</v>
       </c>
     </row>
-    <row r="585" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A585" t="s">
-        <v>693</v>
-      </c>
-      <c r="B585" t="str">
-        <f>_xlfn.TEXTJOIN("|",TRUE,U73:U579)</f>
-        <v>agriculture_kstoggle^1|agriculture_steep^21|architecture_kstoggle^1|architecture_steep^43||astronomy_kstoggle^1|astronomy_steep^24||cryptography_kstoggle^1|cryptography_steep^24||economicsfinanceinvesting_kstoggle^1|economicsfinanceinvesting_steep^30||foreignlanguage_kstoggle^1|foreignlanguage_steep^34||hypnotism_kstoggle^1|hypnotism_steep^14||journalism_kstoggle^1|journalism_steep^18||lipreadingsignlanguage_kstoggle^1|lipreadingsignlanguage_steep^42||nativetongue_kstoggle^1|nativetongue_steep^37||tradelanguage_kstoggle^1|tradelanguage_steep^24||combathandweapons_kstoggle^1|combathandweapons_steep^24||culturedpalate_kstoggle^1|culturedpalate_steep^52||hekaforging_kstoggle^1|hekaforging_steep^32||music_kstoggle^1|music_steep^23||perceptionphysical_kstoggle^1|perceptionphysical_steep^53||sports_kstoggle^1|sports_steep^34||weaponsspecialskill_kstoggle^1|weaponsspecialskill_steep^57||philosophy_kstoggle^1|philosophy_steep^20||streetwise_kstoggle^1|streetwise_steep^32|</v>
-      </c>
-    </row>
     <row r="586" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A586" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="B586" t="str">
-        <f>_xlfn.TEXTJOIN("|",TRUE,V73:V579)</f>
-        <v>animalhusbandry_has^1|floraculture_has^1|economics_has^1|mercantilism_has^1|axe_has^1|onehandedswords_has^1|beverages_has^1|wineswinemaking_has^1|beersbrewing_has^1|spirits_has^1|perfumes_has^1|gourmetmealpreparation_has^1|enhancedobjectquality_has^1|enchantedmechanisms_has^1|hekareservoirs_has^1|keyboards_has^1|stringedbowed_has^1|noticingp_has^1|hearing_has^1|searching_has^1|tracking_has^1|individualnonviolentsports_has^1|florentine_has^1|fastdraw_has^1|specifictarget_has^1|blindfighting_has^1</v>
+        <f>_xlfn.TEXTJOIN("|",TRUE,U73:U580)</f>
+        <v>agriculture_kstoggle^1|agriculture_steep^21|architecture_kstoggle^1|architecture_steep^43||astronomy_kstoggle^1|astronomy_steep^24||cryptography_kstoggle^1|cryptography_steep^24||economicsfinanceinvesting_kstoggle^1|economicsfinanceinvesting_steep^30||foreignlanguage_kstoggle^1|foreignlanguage_steep^34||hypnotism_kstoggle^1|hypnotism_steep^14||journalism_kstoggle^1|journalism_steep^18||lipreadingsignlanguage_kstoggle^1|lipreadingsignlanguage_steep^42||nativetongue_kstoggle^1|nativetongue_steep^37||tradelanguage_kstoggle^1|tradelanguage_steep^24||combathandweapons_kstoggle^1|combathandweapons_steep^24||culturedpalate_kstoggle^1|culturedpalate_steep^52||hekaforging_kstoggle^1|hekaforging_steep^32||music_kstoggle^1|music_steep^23||perceptionphysical_kstoggle^1|perceptionphysical_steep^53||sports_kstoggle^1|sports_steep^34||weaponsspecialskill_kstoggle^1|weaponsspecialskill_steep^57||philosophy_kstoggle^1|philosophy_steep^20||streetwise_kstoggle^1|streetwise_steep^32|</v>
       </c>
     </row>
     <row r="587" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A587" t="s">
+        <v>694</v>
+      </c>
+      <c r="B587" t="str">
+        <f>_xlfn.TEXTJOIN("|",TRUE,V73:V580)</f>
+        <v>animalhusbandry_has^1|floraculture_has^1|economics_has^1|mercantilism_has^1|axe_has^1|onehandedswords_has^1|beverages_has^1|wineswinemaking_has^1|beersbrewing_has^1|spirits_has^1|perfumes_has^1|gourmetmealpreparation_has^1|enhancedobjectquality_has^1|enchantedmechanisms_has^1|hekareservoirs_has^1|keyboards_has^1|stringedbowed_has^1|noticingp_has^1|hearing_has^1|searching_has^1|tracking_has^1|individualnonviolentsports_has^1|florentine_has^1|fastdraw_has^1|specifictarget_has^1|blindfighting_has^1</v>
+      </c>
+    </row>
+    <row r="588" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A588" t="s">
         <v>365</v>
       </c>
-      <c r="B587" t="str">
-        <f>CONCATENATE("merccoms^",E144,"|","languages^",E162,"|","signlanguages^",E208,"|","nativetongue_language^",E215,"|","tradelanguage_language^",E237,"|","florentineweaps^",E449,"|","fastdrawweaps^",E450,"|","specifictargetweaps^",E451,"|","blindfightingweaps^",E452,"|","streetwisesubs^",E575,"|")</f>
+      <c r="B588" t="str">
+        <f>CONCATENATE("merccoms^",E144,"|","languages^",E162,"|","signlanguages^",E208,"|","nativetongue_language^",E215,"|","tradelanguage_language^",E237,"|","florentineweaps^",E450,"|","fastdrawweaps^",E451,"|","specifictargetweaps^",E452,"|","blindfightingweaps^",E453,"|","streetwisesubs^",E576,"|")</f>
         <v>merccoms^Furs,Silver|languages^French:34,Deutsch:58|signlanguages^Romani,Tramps,Thieves|nativetongue_language^Atlantlan|tradelanguage_language^Trade Phoenecian|florentineweaps^axe,onehandedswords|fastdrawweaps^whipflail,axe|specifictargetweaps^axe|blindfightingweaps^poleaxe|streetwisesubs^Merchants,Artists,Gangs|</v>
       </c>
     </row>
-    <row r="589" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A589" s="9" t="s">
+    <row r="590" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A590" s="9" t="s">
         <v>695</v>
       </c>
-      <c r="B589" s="4" t="str">
-        <f>CONCATENATE(B584,"|",B585,"|",B586,"|",B587)</f>
+      <c r="B590" s="4" t="str">
+        <f>CONCATENATE(B585,"|",B586,"|",B587,"|",B588)</f>
         <v>character_name^Smartypants Hottieface|vocation^Seafarer|vocationtrait^PHYSICAL|sec^5|attractiveness^18|beautyugly^|ap^2|joss^3|mmcapatt^19|mmpowatt^14|mmspdatt^18|mrcapatt^15|mrpowatt^12|mrspdatt^11|pmcapatt^20|pmpowatt^19|pmspdatt^15|pncapatt^19|pnpowatt^18|pnspdatt^17|smcapatt^16|smpowatt^12|smspdatt^11|spcapatt^15|sppowatt^12|spspdatt^13|traithekamental_toggle^0|traithekaphysical_toggle^1|traithekaspiritual_toggle^0|fpdweomer^0|fppriest^0|dweomerschool^|priestethos^|vowpact^|vowpact_mult^1|age^18|sex^Indeed|race^Faerie|complexion^Mocha|handedness^Left|height^5'6"|weight^145 lb.|build^Brickhouse|eyes^Blue|hair^Black|physicalother^Svelte|personality^Savage|quirks^|quote^|birthdate^|birthplace^|birthrank^|citizenship^Detroit|residence^Arizona|background^|connections^|networth^|bankaccounts^|cashonhand^|dmi^|possessions1^|agriculture_kstoggle^1|agriculture_steep^21|architecture_kstoggle^1|architecture_steep^43||astronomy_kstoggle^1|astronomy_steep^24||cryptography_kstoggle^1|cryptography_steep^24||economicsfinanceinvesting_kstoggle^1|economicsfinanceinvesting_steep^30||foreignlanguage_kstoggle^1|foreignlanguage_steep^34||hypnotism_kstoggle^1|hypnotism_steep^14||journalism_kstoggle^1|journalism_steep^18||lipreadingsignlanguage_kstoggle^1|lipreadingsignlanguage_steep^42||nativetongue_kstoggle^1|nativetongue_steep^37||tradelanguage_kstoggle^1|tradelanguage_steep^24||combathandweapons_kstoggle^1|combathandweapons_steep^24||culturedpalate_kstoggle^1|culturedpalate_steep^52||hekaforging_kstoggle^1|hekaforging_steep^32||music_kstoggle^1|music_steep^23||perceptionphysical_kstoggle^1|perceptionphysical_steep^53||sports_kstoggle^1|sports_steep^34||weaponsspecialskill_kstoggle^1|weaponsspecialskill_steep^57||philosophy_kstoggle^1|philosophy_steep^20||streetwise_kstoggle^1|streetwise_steep^32||animalhusbandry_has^1|floraculture_has^1|economics_has^1|mercantilism_has^1|axe_has^1|onehandedswords_has^1|beverages_has^1|wineswinemaking_has^1|beersbrewing_has^1|spirits_has^1|perfumes_has^1|gourmetmealpreparation_has^1|enhancedobjectquality_has^1|enchantedmechanisms_has^1|hekareservoirs_has^1|keyboards_has^1|stringedbowed_has^1|noticingp_has^1|hearing_has^1|searching_has^1|tracking_has^1|individualnonviolentsports_has^1|florentine_has^1|fastdraw_has^1|specifictarget_has^1|blindfighting_has^1|merccoms^Furs,Silver|languages^French:34,Deutsch:58|signlanguages^Romani,Tramps,Thieves|nativetongue_language^Atlantlan|tradelanguage_language^Trade Phoenecian|florentineweaps^axe,onehandedswords|fastdrawweaps^whipflail,axe|specifictargetweaps^axe|blindfightingweaps^poleaxe|streetwisesubs^Merchants,Artists,Gangs|</v>
       </c>
     </row>

</xml_diff>